<commit_message>
Update documentation with new releases
</commit_message>
<xml_diff>
--- a/docs/_static/xlsx/tab_Esenzione_bollo.xlsx
+++ b/docs/_static/xlsx/tab_Esenzione_bollo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>SI</t>
+  </si>
+  <si>
+    <t>ALTRO MOTIVO DI ESENZIONE</t>
   </si>
 </sst>
 </file>
@@ -417,11 +420,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -547,6 +550,14 @@
         <v>16</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>99</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>